<commit_message>
fix original map + update xlsx
</commit_message>
<xml_diff>
--- a/charts.xlsx
+++ b/charts.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projet\Projet_CESI\2025-2026\IR\Projets\Mario-AI-Framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2524CC-AC60-4DB2-A5B6-7F2BBFF9CD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD98DBD-B82B-4309-8812-259FD7E68840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="log (2)" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil1" sheetId="3" r:id="rId2"/>
+    <sheet name="Generated" sheetId="1" r:id="rId1"/>
+    <sheet name="generatedEch" sheetId="3" r:id="rId2"/>
     <sheet name="log (3)" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="DonnéesExternes_1" localSheetId="0" hidden="1">'log (2)'!#REF!</definedName>
+    <definedName name="DonnéesExternes_1" localSheetId="0" hidden="1">Generated!#REF!</definedName>
     <definedName name="DonnéesExternes_1" localSheetId="2" hidden="1">'log (3)'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1920" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1926" uniqueCount="343">
   <si>
     <t>LevelPath</t>
   </si>
@@ -1428,7 +1428,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'log (2)'!$B$256:$B$258</c:f>
+              <c:f>Generated!$B$256:$B$258</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1445,7 +1445,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'log (2)'!$C$256:$C$258</c:f>
+              <c:f>Generated!$C$256:$C$258</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1615,7 +1615,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'log (2)'!$B$256:$B$258</c:f>
+              <c:f>Generated!$B$256:$B$258</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1632,7 +1632,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'log (2)'!$C$256:$C$258</c:f>
+              <c:f>Generated!$C$256:$C$258</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1985,7 +1985,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'log (2)'!$B$262:$B$264</c:f>
+              <c:f>Generated!$B$262:$B$264</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2002,7 +2002,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'log (2)'!$C$262:$C$264</c:f>
+              <c:f>Generated!$C$262:$C$264</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2360,7 +2360,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'log (2)'!$B$256:$B$258</c:f>
+              <c:f>Generated!$B$256:$B$258</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2377,7 +2377,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'log (2)'!$C$256:$C$258</c:f>
+              <c:f>Generated!$C$256:$C$258</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2547,7 +2547,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'log (2)'!$B$256:$B$258</c:f>
+              <c:f>Generated!$B$256:$B$258</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2564,7 +2564,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'log (2)'!$C$256:$C$258</c:f>
+              <c:f>Generated!$C$256:$C$258</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2917,7 +2917,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'log (2)'!$B$262:$B$264</c:f>
+              <c:f>Generated!$B$262:$B$264</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2934,7 +2934,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'log (2)'!$C$262:$C$264</c:f>
+              <c:f>Generated!$C$262:$C$264</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -8122,10 +8122,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2598870A-4957-49A8-9407-B48E29DBA94C}" name="log_3" displayName="log_3" ref="A1:O17" totalsRowShown="0">
-  <autoFilter ref="A1:O17" xr:uid="{2598870A-4957-49A8-9407-B48E29DBA94C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O17">
-    <sortCondition descending="1" ref="B1:B17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2598870A-4957-49A8-9407-B48E29DBA94C}" name="log_3" displayName="log_3" ref="A1:O19" totalsRowShown="0">
+  <autoFilter ref="A1:O19" xr:uid="{2598870A-4957-49A8-9407-B48E29DBA94C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O19">
+    <sortCondition ref="B1:B19"/>
   </sortState>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{F8FA52C7-0BC3-4ABC-848E-179E64C0C5F3}" name="LevelPath"/>
@@ -8355,8 +8355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA265"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77:XFD77"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H143" sqref="A143:XFD143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19881,7 +19881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="142" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>235</v>
       </c>
@@ -29318,8 +29318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD19E77-9812-437A-83B1-09A57173861D}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29390,10 +29390,10 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -29402,31 +29402,31 @@
         <v>100</v>
       </c>
       <c r="E2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F2">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G2">
-        <v>218.18</v>
+        <v>218.75</v>
       </c>
       <c r="H2">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>-96</v>
+        <v>-43</v>
       </c>
       <c r="K2">
-        <v>3.7908059999999999</v>
+        <v>0.97326000000000001</v>
       </c>
       <c r="L2">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="M2">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -29437,10 +29437,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
@@ -29449,81 +29449,81 @@
         <v>100</v>
       </c>
       <c r="E3">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="G3">
-        <v>141.82</v>
+        <v>410.82</v>
       </c>
       <c r="H3">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="I3">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>-71</v>
+        <v>-121</v>
       </c>
       <c r="K3">
-        <v>2.1273819999999999</v>
+        <v>4.2734269999999999</v>
       </c>
       <c r="L3">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="M3">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="N3">
         <v>0</v>
       </c>
       <c r="O3">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="D4">
-        <v>100</v>
+        <v>37.89</v>
       </c>
       <c r="E4">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="G4">
-        <v>152.72999999999999</v>
+        <v>131.41</v>
       </c>
       <c r="H4">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0.59</v>
       </c>
       <c r="J4">
-        <v>-43</v>
+        <v>-41</v>
       </c>
       <c r="K4">
-        <v>0.97326000000000001</v>
+        <v>0.91326200000000002</v>
       </c>
       <c r="L4">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="M4">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O4">
         <v>8</v>
@@ -29531,49 +29531,49 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>290</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="D5">
-        <v>100</v>
+        <v>29.12</v>
       </c>
       <c r="E5">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="G5">
-        <v>207.27</v>
+        <v>129.63999999999999</v>
       </c>
       <c r="H5">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I5">
-        <v>0.18</v>
+        <v>1</v>
       </c>
       <c r="J5">
-        <v>-67</v>
+        <v>-86</v>
       </c>
       <c r="K5">
-        <v>2.7204290000000002</v>
+        <v>3.7367970000000001</v>
       </c>
       <c r="L5">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="M5">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="N5">
         <v>0</v>
       </c>
       <c r="O5">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -29581,25 +29581,25 @@
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
         <v>31</v>
       </c>
       <c r="D6">
-        <v>93.4</v>
+        <v>77.489999999999995</v>
       </c>
       <c r="E6">
         <v>14</v>
       </c>
       <c r="F6">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G6">
-        <v>163.58000000000001</v>
+        <v>129.63999999999999</v>
       </c>
       <c r="H6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I6">
         <v>0.99</v>
@@ -29625,46 +29625,46 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
         <v>31</v>
       </c>
       <c r="D7">
-        <v>68.599999999999994</v>
+        <v>34.58</v>
       </c>
       <c r="E7">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G7">
-        <v>124.07</v>
+        <v>129.63999999999999</v>
       </c>
       <c r="H7">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I7">
-        <v>0.59</v>
+        <v>1</v>
       </c>
       <c r="J7">
-        <v>-41</v>
+        <v>-96</v>
       </c>
       <c r="K7">
-        <v>0.91326200000000002</v>
+        <v>3.7908059999999999</v>
       </c>
       <c r="L7">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="M7">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="N7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O7">
         <v>8</v>
@@ -29672,137 +29672,137 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
         <v>31</v>
       </c>
       <c r="D8">
-        <v>66.19</v>
+        <v>34.18</v>
       </c>
       <c r="E8">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F8">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G8">
-        <v>119.71</v>
+        <v>129.63999999999999</v>
       </c>
       <c r="H8">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0.18</v>
       </c>
       <c r="J8">
-        <v>-86</v>
+        <v>-67</v>
       </c>
       <c r="K8">
-        <v>3.7367970000000001</v>
+        <v>2.7204290000000002</v>
       </c>
       <c r="L8">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="M8">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="N8">
         <v>0</v>
       </c>
       <c r="O8">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
         <v>31</v>
       </c>
       <c r="D9">
-        <v>65.28</v>
+        <v>32.94</v>
       </c>
       <c r="E9">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F9">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G9">
-        <v>239.88</v>
+        <v>129.63999999999999</v>
       </c>
       <c r="H9">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="J9">
-        <v>-163</v>
+        <v>-71</v>
       </c>
       <c r="K9">
-        <v>9.2431970000000003</v>
+        <v>2.1273819999999999</v>
       </c>
       <c r="L9">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="M9">
-        <v>176</v>
+        <v>52</v>
       </c>
       <c r="N9">
         <v>0</v>
       </c>
       <c r="O9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
         <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D10">
-        <v>100</v>
+        <v>16.89</v>
       </c>
       <c r="E10">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F10">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="G10">
-        <v>218.75</v>
+        <v>129.63999999999999</v>
       </c>
       <c r="H10">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10">
-        <v>-43</v>
+        <v>-163</v>
       </c>
       <c r="K10">
-        <v>0.97326000000000001</v>
+        <v>9.2431970000000003</v>
       </c>
       <c r="L10">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="M10">
-        <v>37</v>
+        <v>176</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -29813,46 +29813,46 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="D11">
-        <v>37.89</v>
+        <v>100</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F11">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="G11">
-        <v>131.41</v>
+        <v>218.18</v>
       </c>
       <c r="H11">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I11">
-        <v>0.59</v>
+        <v>1</v>
       </c>
       <c r="J11">
-        <v>-41</v>
+        <v>-96</v>
       </c>
       <c r="K11">
-        <v>0.91326200000000002</v>
+        <v>3.7908059999999999</v>
       </c>
       <c r="L11">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="M11">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="N11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O11">
         <v>8</v>
@@ -29860,137 +29860,137 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="D12">
-        <v>29.12</v>
+        <v>100</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F12">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="G12">
-        <v>129.63999999999999</v>
+        <v>141.82</v>
       </c>
       <c r="H12">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="J12">
-        <v>-86</v>
+        <v>-71</v>
       </c>
       <c r="K12">
-        <v>3.7367970000000001</v>
+        <v>2.1273819999999999</v>
       </c>
       <c r="L12">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="M12">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="N12">
         <v>0</v>
       </c>
       <c r="O12">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D13">
-        <v>77.489999999999995</v>
+        <v>100</v>
       </c>
       <c r="E13">
         <v>14</v>
       </c>
       <c r="F13">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G13">
-        <v>129.63999999999999</v>
+        <v>152.72999999999999</v>
       </c>
       <c r="H13">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I13">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="J13">
-        <v>-59</v>
+        <v>-43</v>
       </c>
       <c r="K13">
-        <v>1.7955559999999999</v>
+        <v>0.97326000000000001</v>
       </c>
       <c r="L13">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M13">
         <v>37</v>
       </c>
       <c r="N13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O13">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>290</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D14">
-        <v>34.58</v>
+        <v>100</v>
       </c>
       <c r="E14">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F14">
         <v>9</v>
       </c>
       <c r="G14">
-        <v>129.63999999999999</v>
+        <v>207.27</v>
       </c>
       <c r="H14">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I14">
-        <v>1</v>
+        <v>0.18</v>
       </c>
       <c r="J14">
-        <v>-96</v>
+        <v>-67</v>
       </c>
       <c r="K14">
-        <v>3.7908059999999999</v>
+        <v>2.7204290000000002</v>
       </c>
       <c r="L14">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M14">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="N14">
         <v>0</v>
@@ -30001,142 +30001,236 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>308</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D15">
-        <v>34.18</v>
+        <v>100</v>
       </c>
       <c r="E15">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F15">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G15">
-        <v>129.63999999999999</v>
+        <v>174.54</v>
       </c>
       <c r="H15">
         <v>15</v>
       </c>
       <c r="I15">
-        <v>0.18</v>
+        <v>1</v>
       </c>
       <c r="J15">
-        <v>-67</v>
+        <v>-121</v>
       </c>
       <c r="K15">
-        <v>2.7204290000000002</v>
+        <v>4.2734269999999999</v>
       </c>
       <c r="L15">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="M15">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="N15">
         <v>0</v>
       </c>
       <c r="O15">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
         <v>31</v>
       </c>
       <c r="D16">
-        <v>32.94</v>
+        <v>93.4</v>
       </c>
       <c r="E16">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F16">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G16">
-        <v>129.63999999999999</v>
+        <v>163.58000000000001</v>
       </c>
       <c r="H16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I16">
-        <v>0.97</v>
+        <v>0.99</v>
       </c>
       <c r="J16">
-        <v>-71</v>
+        <v>-59</v>
       </c>
       <c r="K16">
-        <v>2.1273819999999999</v>
+        <v>1.7955559999999999</v>
       </c>
       <c r="L16">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M16">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O16">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
         <v>31</v>
       </c>
       <c r="D17">
-        <v>16.89</v>
+        <v>68.599999999999994</v>
       </c>
       <c r="E17">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F17">
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <v>124.07</v>
+      </c>
+      <c r="H17">
+        <v>14</v>
+      </c>
+      <c r="I17">
+        <v>0.59</v>
+      </c>
+      <c r="J17">
+        <v>-41</v>
+      </c>
+      <c r="K17">
+        <v>0.91326200000000002</v>
+      </c>
+      <c r="L17">
+        <v>11</v>
+      </c>
+      <c r="M17">
+        <v>21</v>
+      </c>
+      <c r="N17">
+        <v>2</v>
+      </c>
+      <c r="O17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18">
+        <v>66.19</v>
+      </c>
+      <c r="E18">
+        <v>16</v>
+      </c>
+      <c r="F18">
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <v>119.71</v>
+      </c>
+      <c r="H18">
+        <v>10</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>-86</v>
+      </c>
+      <c r="K18">
+        <v>3.7367970000000001</v>
+      </c>
+      <c r="L18">
+        <v>32</v>
+      </c>
+      <c r="M18">
+        <v>70</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19">
+        <v>65.28</v>
+      </c>
+      <c r="E19">
+        <v>16</v>
+      </c>
+      <c r="F19">
         <v>5</v>
       </c>
-      <c r="G17">
-        <v>129.63999999999999</v>
-      </c>
-      <c r="H17">
-        <v>15</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="J17">
+      <c r="G19">
+        <v>239.88</v>
+      </c>
+      <c r="H19">
+        <v>21</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
         <v>-163</v>
       </c>
-      <c r="K17">
+      <c r="K19">
         <v>9.2431970000000003</v>
       </c>
-      <c r="L17">
+      <c r="L19">
         <v>65</v>
       </c>
-      <c r="M17">
+      <c r="M19">
         <v>176</v>
       </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17">
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
         <v>8</v>
       </c>
     </row>
@@ -30156,12 +30250,12 @@
         <v>29</v>
       </c>
       <c r="C35">
-        <f>COUNTIF(C2:C17,"WIN")</f>
-        <v>5</v>
+        <f>COUNTIF(C2:C19,"WIN")</f>
+        <v>7</v>
       </c>
       <c r="D35">
-        <f>AVERAGE(D2:D17)</f>
-        <v>66.035000000000011</v>
+        <f>AVERAGE(D2:D19)</f>
+        <v>69.808888888888887</v>
       </c>
       <c r="J35" t="e">
         <f>AVERAGEA(#REF!)</f>
@@ -30173,7 +30267,7 @@
         <v>31</v>
       </c>
       <c r="C36">
-        <f>COUNTIF(C2:C17,"LOSE")</f>
+        <f>COUNTIF(C2:C19,"LOSE")</f>
         <v>9</v>
       </c>
       <c r="J36" t="e">
@@ -30186,7 +30280,7 @@
         <v>45</v>
       </c>
       <c r="C37">
-        <f>COUNTIF(C2:C17,"TIME_OUT")</f>
+        <f>COUNTIF(C2:C19,"TIME_OUT")</f>
         <v>2</v>
       </c>
     </row>
@@ -30196,7 +30290,7 @@
       </c>
       <c r="C38">
         <f>SUM(C35:C37)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -30244,7 +30338,275 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D17">
+  <conditionalFormatting sqref="D2:D19">
+    <cfRule type="colorScale" priority="187">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D5">
+    <cfRule type="colorScale" priority="172">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6:D7">
+    <cfRule type="colorScale" priority="157">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:D9">
+    <cfRule type="colorScale" priority="127">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:D11">
+    <cfRule type="colorScale" priority="112">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:D13">
+    <cfRule type="colorScale" priority="97">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14:D15">
+    <cfRule type="colorScale" priority="82">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="colorScale" priority="61">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34:D1048576 D1">
+    <cfRule type="colorScale" priority="209">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:N19">
+    <cfRule type="colorScale" priority="708">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:N5">
+    <cfRule type="colorScale" priority="710">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6:N7">
+    <cfRule type="colorScale" priority="712">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:N9">
+    <cfRule type="colorScale" priority="714">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:N11">
+    <cfRule type="colorScale" priority="716">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:N13">
+    <cfRule type="colorScale" priority="718">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14:N15">
+    <cfRule type="colorScale" priority="720">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:N16">
+    <cfRule type="colorScale" priority="722">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17:N17">
+    <cfRule type="colorScale" priority="724">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34:O1048576 D1:N1">
+    <cfRule type="colorScale" priority="704">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E19">
+    <cfRule type="colorScale" priority="177">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="178">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E5">
+    <cfRule type="colorScale" priority="162">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="163">
       <colorScale>
         <cfvo type="min"/>
@@ -30256,7 +30618,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D5">
+  <conditionalFormatting sqref="E6:E7">
+    <cfRule type="colorScale" priority="147">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="148">
       <colorScale>
         <cfvo type="min"/>
@@ -30268,8 +30638,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6:D7">
-    <cfRule type="colorScale" priority="133">
+  <conditionalFormatting sqref="E8:E9">
+    <cfRule type="colorScale" priority="117">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="118">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -30280,7 +30658,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D9">
+  <conditionalFormatting sqref="E10:E11">
+    <cfRule type="colorScale" priority="102">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="103">
       <colorScale>
         <cfvo type="min"/>
@@ -30292,7 +30678,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10:D11">
+  <conditionalFormatting sqref="E12:E13">
+    <cfRule type="colorScale" priority="87">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="88">
       <colorScale>
         <cfvo type="min"/>
@@ -30304,7 +30698,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D12:D13">
+  <conditionalFormatting sqref="E14:E15">
+    <cfRule type="colorScale" priority="72">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="73">
       <colorScale>
         <cfvo type="min"/>
@@ -30316,8 +30718,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14:D15">
-    <cfRule type="colorScale" priority="58">
+  <conditionalFormatting sqref="E16">
+    <cfRule type="colorScale" priority="51">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -30328,7 +30738,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
+  <conditionalFormatting sqref="E17">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -30340,8 +30758,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
-    <cfRule type="colorScale" priority="22">
+  <conditionalFormatting sqref="E34:E1048576 E1">
+    <cfRule type="colorScale" priority="213">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="217">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -30352,8 +30778,470 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34:D1048576 D1">
-    <cfRule type="colorScale" priority="185">
+  <conditionalFormatting sqref="F2:F19">
+    <cfRule type="colorScale" priority="176">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="179">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:F5">
+    <cfRule type="colorScale" priority="161">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="164">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6:F7">
+    <cfRule type="colorScale" priority="146">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="149">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8:F9">
+    <cfRule type="colorScale" priority="116">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="119">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10:F11">
+    <cfRule type="colorScale" priority="101">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="104">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12:F13">
+    <cfRule type="colorScale" priority="86">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="89">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14:F15">
+    <cfRule type="colorScale" priority="71">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="74">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16">
+    <cfRule type="colorScale" priority="50">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="53">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F34:F1048576 F1">
+    <cfRule type="colorScale" priority="221">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="225">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H19 H22:H1048576">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H19">
+    <cfRule type="colorScale" priority="180">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H5">
+    <cfRule type="colorScale" priority="165">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6:H7">
+    <cfRule type="colorScale" priority="150">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8:H9">
+    <cfRule type="colorScale" priority="120">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10:H11">
+    <cfRule type="colorScale" priority="105">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12:H13">
+    <cfRule type="colorScale" priority="90">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14:H15">
+    <cfRule type="colorScale" priority="75">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16">
+    <cfRule type="colorScale" priority="54">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34:H1048576 H1">
+    <cfRule type="colorScale" priority="229">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I19">
+    <cfRule type="colorScale" priority="181">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:I5">
+    <cfRule type="colorScale" priority="166">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6:I7">
+    <cfRule type="colorScale" priority="151">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8:I9">
+    <cfRule type="colorScale" priority="121">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10:I11">
+    <cfRule type="colorScale" priority="106">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12:I13">
+    <cfRule type="colorScale" priority="91">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:I15">
+    <cfRule type="colorScale" priority="76">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="colorScale" priority="55">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22:I1048576">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I34:I1048576">
+    <cfRule type="colorScale" priority="608">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:J15 K22:K1048576">
+    <cfRule type="colorScale" priority="68">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -30364,16 +31252,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E17">
-    <cfRule type="colorScale" priority="153">
+  <conditionalFormatting sqref="J34:J1048576 I1">
+    <cfRule type="colorScale" priority="237">
       <colorScale>
         <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="154">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:K15 L22:L1048576">
+    <cfRule type="colorScale" priority="67">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -30384,195 +31276,295 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E5">
-    <cfRule type="colorScale" priority="138">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="139">
+  <conditionalFormatting sqref="K2:K19">
+    <cfRule type="colorScale" priority="186">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E6:E7">
-    <cfRule type="colorScale" priority="123">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="124">
+  <conditionalFormatting sqref="K4:K5">
+    <cfRule type="colorScale" priority="171">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8:E9">
-    <cfRule type="colorScale" priority="93">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="94">
+  <conditionalFormatting sqref="K6:K7">
+    <cfRule type="colorScale" priority="156">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10:E11">
-    <cfRule type="colorScale" priority="78">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="79">
+  <conditionalFormatting sqref="K8:K9">
+    <cfRule type="colorScale" priority="126">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12:E13">
-    <cfRule type="colorScale" priority="63">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="64">
+  <conditionalFormatting sqref="K10:K11">
+    <cfRule type="colorScale" priority="111">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E15">
-    <cfRule type="colorScale" priority="48">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="49">
+  <conditionalFormatting sqref="K12:K13">
+    <cfRule type="colorScale" priority="96">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E16">
-    <cfRule type="colorScale" priority="27">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="28">
+  <conditionalFormatting sqref="K14:K15">
+    <cfRule type="colorScale" priority="81">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="13">
+  <conditionalFormatting sqref="K16">
+    <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E34:E1048576 E1">
-    <cfRule type="colorScale" priority="189">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="193">
+  <conditionalFormatting sqref="K17">
+    <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F17">
+  <conditionalFormatting sqref="L1:L15 M22:M1048576">
+    <cfRule type="colorScale" priority="66">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L19">
+    <cfRule type="colorScale" priority="182">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4:L5">
+    <cfRule type="colorScale" priority="167">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L6:L7">
     <cfRule type="colorScale" priority="152">
       <colorScale>
         <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L8:L9">
+    <cfRule type="colorScale" priority="122">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L10:L11">
+    <cfRule type="colorScale" priority="107">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L12:L13">
+    <cfRule type="colorScale" priority="92">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L14:L15">
+    <cfRule type="colorScale" priority="77">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L16">
+    <cfRule type="colorScale" priority="56">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L17">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:K19 L22:L1048576">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L34:L1048576 K1">
+    <cfRule type="colorScale" priority="241">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M1:M15 N22:N1048576">
+    <cfRule type="colorScale" priority="65">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M19">
+    <cfRule type="colorScale" priority="185">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M4:M5">
+    <cfRule type="colorScale" priority="170">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M6:M7">
     <cfRule type="colorScale" priority="155">
       <colorScale>
         <cfvo type="min"/>
@@ -30584,35 +31576,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:F5">
-    <cfRule type="colorScale" priority="137">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="140">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F6:F7">
-    <cfRule type="colorScale" priority="122">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
+  <conditionalFormatting sqref="M8:M9">
     <cfRule type="colorScale" priority="125">
       <colorScale>
         <cfvo type="min"/>
@@ -30624,15 +31588,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F8:F9">
-    <cfRule type="colorScale" priority="92">
+  <conditionalFormatting sqref="M10:M11">
+    <cfRule type="colorScale" priority="110">
       <colorScale>
         <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M12:M13">
     <cfRule type="colorScale" priority="95">
       <colorScale>
         <cfvo type="min"/>
@@ -30644,15 +31612,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F10:F11">
-    <cfRule type="colorScale" priority="77">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
+  <conditionalFormatting sqref="M14:M15">
     <cfRule type="colorScale" priority="80">
       <colorScale>
         <cfvo type="min"/>
@@ -30664,16 +31624,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F12:F13">
-    <cfRule type="colorScale" priority="62">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="65">
+  <conditionalFormatting sqref="M16">
+    <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -30684,16 +31636,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F14:F15">
-    <cfRule type="colorScale" priority="47">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="50">
+  <conditionalFormatting sqref="M17">
+    <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -30704,560 +31648,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F16">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F17">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F34:F1048576 F1">
-    <cfRule type="colorScale" priority="197">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="201">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H17">
-    <cfRule type="colorScale" priority="156">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H5">
-    <cfRule type="colorScale" priority="141">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H6:H7">
-    <cfRule type="colorScale" priority="126">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H8:H9">
-    <cfRule type="colorScale" priority="96">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10:H11">
-    <cfRule type="colorScale" priority="81">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H12:H13">
-    <cfRule type="colorScale" priority="66">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H14:H15">
-    <cfRule type="colorScale" priority="51">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16">
-    <cfRule type="colorScale" priority="30">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H17">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H34:H1048576 H1">
-    <cfRule type="colorScale" priority="205">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I17">
-    <cfRule type="colorScale" priority="157">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4:I5">
-    <cfRule type="colorScale" priority="142">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6:I7">
-    <cfRule type="colorScale" priority="127">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8:I9">
-    <cfRule type="colorScale" priority="97">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I10:I11">
-    <cfRule type="colorScale" priority="82">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12:I13">
-    <cfRule type="colorScale" priority="67">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14:I15">
-    <cfRule type="colorScale" priority="52">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
-    <cfRule type="colorScale" priority="31">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J34:J1048576 I1">
-    <cfRule type="colorScale" priority="213">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J15 K18:K1048576">
-    <cfRule type="colorScale" priority="44">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K15 L18:L1048576">
-    <cfRule type="colorScale" priority="43">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K17">
-    <cfRule type="colorScale" priority="162">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4:K5">
-    <cfRule type="colorScale" priority="147">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K6:K7">
-    <cfRule type="colorScale" priority="132">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K8:K9">
-    <cfRule type="colorScale" priority="102">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10:K11">
-    <cfRule type="colorScale" priority="87">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K12:K13">
-    <cfRule type="colorScale" priority="72">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K14:K15">
-    <cfRule type="colorScale" priority="57">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K16">
-    <cfRule type="colorScale" priority="36">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K17">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L34:L1048576 K1">
-    <cfRule type="colorScale" priority="217">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L15 M18:M1048576">
-    <cfRule type="colorScale" priority="42">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L17">
-    <cfRule type="colorScale" priority="158">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L4:L5">
-    <cfRule type="colorScale" priority="143">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L6:L7">
-    <cfRule type="colorScale" priority="128">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L8:L9">
-    <cfRule type="colorScale" priority="98">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L10:L11">
-    <cfRule type="colorScale" priority="83">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L12:L13">
-    <cfRule type="colorScale" priority="68">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L14:L15">
-    <cfRule type="colorScale" priority="53">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L16">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L17">
-    <cfRule type="colorScale" priority="17">
+  <conditionalFormatting sqref="L1:L19 M22:M1048576">
+    <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31269,7 +31661,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M34:M1048576 L1">
-    <cfRule type="colorScale" priority="221">
+    <cfRule type="colorScale" priority="245">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31280,8 +31672,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M15 N18:N1048576">
-    <cfRule type="colorScale" priority="41">
+  <conditionalFormatting sqref="N1:N15 O22:O1048576">
+    <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31292,140 +31684,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M17">
-    <cfRule type="colorScale" priority="161">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M4:M5">
-    <cfRule type="colorScale" priority="146">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M6:M7">
-    <cfRule type="colorScale" priority="131">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M8:M9">
-    <cfRule type="colorScale" priority="101">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M10:M11">
-    <cfRule type="colorScale" priority="86">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M12:M13">
-    <cfRule type="colorScale" priority="71">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M14:M15">
-    <cfRule type="colorScale" priority="56">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M16">
-    <cfRule type="colorScale" priority="35">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M17">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N34:N1048576 M1">
-    <cfRule type="colorScale" priority="225">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N15 O18:O1048576">
-    <cfRule type="colorScale" priority="40">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N17">
-    <cfRule type="colorScale" priority="160">
+  <conditionalFormatting sqref="N2:N19">
+    <cfRule type="colorScale" priority="184">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31437,7 +31697,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:N5">
-    <cfRule type="colorScale" priority="145">
+    <cfRule type="colorScale" priority="169">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31449,7 +31709,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6:N7">
-    <cfRule type="colorScale" priority="130">
+    <cfRule type="colorScale" priority="154">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31461,7 +31721,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8:N9">
-    <cfRule type="colorScale" priority="100">
+    <cfRule type="colorScale" priority="124">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31473,7 +31733,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10:N11">
-    <cfRule type="colorScale" priority="85">
+    <cfRule type="colorScale" priority="109">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31485,7 +31745,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N12:N13">
-    <cfRule type="colorScale" priority="70">
+    <cfRule type="colorScale" priority="94">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31497,7 +31757,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N14:N15">
-    <cfRule type="colorScale" priority="55">
+    <cfRule type="colorScale" priority="79">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31509,7 +31769,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16">
-    <cfRule type="colorScale" priority="34">
+    <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31521,7 +31781,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17">
-    <cfRule type="colorScale" priority="19">
+    <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31532,8 +31792,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O34:O1048576 N1">
-    <cfRule type="colorScale" priority="229">
+  <conditionalFormatting sqref="M1:M19 N22:N1048576">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31543,31 +31803,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O18:O1048576 N1:N17">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N18:N1048576 M1:M17">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -31576,54 +31812,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M18:M1048576 L1:L17">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L18:L1048576 K1:K17">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18:I1048576">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I34:I1048576">
-    <cfRule type="colorScale" priority="584">
+  <conditionalFormatting sqref="N34:N1048576 M1">
+    <cfRule type="colorScale" priority="249">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31635,7 +31825,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O17">
-    <cfRule type="dataBar" priority="617">
+    <cfRule type="dataBar" priority="641">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -31648,8 +31838,32 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34:O1048576 D1:N1">
-    <cfRule type="colorScale" priority="680">
+  <conditionalFormatting sqref="N1:N19 O22:O1048576">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O34:O1048576 N1">
+    <cfRule type="colorScale" priority="253">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18:D21">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31660,8 +31874,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:N17">
-    <cfRule type="colorScale" priority="684">
+  <conditionalFormatting sqref="E18:E21">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18:E21">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31672,8 +31896,114 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:N5">
-    <cfRule type="colorScale" priority="686">
+  <conditionalFormatting sqref="F18:F21">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18:F21">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18:H21">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18:I21">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18:K21">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L18:L21">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M18:M21">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N18:N21">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O20:O21">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O20:O21">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31684,8 +32014,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6:N7">
-    <cfRule type="colorScale" priority="688">
+  <conditionalFormatting sqref="Q20:S21 D20:O21">
+    <cfRule type="colorScale" priority="817">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31696,8 +32026,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:N9">
-    <cfRule type="colorScale" priority="690">
+  <conditionalFormatting sqref="D18:N19">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -31708,64 +32038,102 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10:N11">
-    <cfRule type="colorScale" priority="692">
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D12:N13">
-    <cfRule type="colorScale" priority="694">
+  <conditionalFormatting sqref="M1:M1048576">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14:N15">
-    <cfRule type="colorScale" priority="696">
+  <conditionalFormatting sqref="N1:N1048576">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16:N16">
-    <cfRule type="colorScale" priority="698">
+  <conditionalFormatting sqref="P11">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2C864B7E-D385-46FA-BE07-A943272DC05E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:K1048576">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17:N17">
-    <cfRule type="colorScale" priority="700">
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O1:O1048576">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{4892D916-0950-4ADB-8382-4C81759E621D}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -31787,6 +32155,32 @@
           </x14:cfRule>
           <xm:sqref>O1:O17</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2C864B7E-D385-46FA-BE07-A943272DC05E}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>P11</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{4892D916-0950-4ADB-8382-4C81759E621D}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>O1:O1048576</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -31797,8 +32191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B542EE2-F317-4A75-B91B-245BC02C5954}">
   <dimension ref="A1:T265"/>
   <sheetViews>
-    <sheetView zoomScale="15" zoomScaleNormal="15" workbookViewId="0">
-      <selection activeCell="AQ137" sqref="AQ137"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N47" sqref="N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44982,6 +45376,18 @@
     </row>
   </sheetData>
   <dataConsolidate/>
+  <conditionalFormatting sqref="D255:D258 D259:Z1048576 F255:Z258 D1:P253">
+    <cfRule type="colorScale" priority="276">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D255:D1048576 D1:D253">
     <cfRule type="colorScale" priority="14">
       <colorScale>
@@ -45146,18 +45552,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D255:D258 D259:Z1048576 F255:Z258 D1:P253">
-    <cfRule type="colorScale" priority="276">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <drawing r:id="rId1"/>

</xml_diff>